<commit_message>
fix database save Load by gameManager
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="objectdatas" sheetId="1" r:id="rId1"/>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1296,7 +1296,7 @@
         <v>200</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -2064,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>